<commit_message>
Carregando dados de Dez/2025
</commit_message>
<xml_diff>
--- a/upload/partos-2025.xlsx
+++ b/upload/partos-2025.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\x17954399\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m10428324\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12180"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Export" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="9">
   <si>
     <t>unidade</t>
   </si>
@@ -372,10 +372,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E45"/>
+  <dimension ref="A1:E193"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47:XFD47"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A194" sqref="A194:XFD195"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -402,16 +402,16 @@
         <v>5</v>
       </c>
       <c r="B2" s="2">
-        <v>2025</v>
+        <v>2022</v>
       </c>
       <c r="C2" s="2">
         <v>1</v>
       </c>
       <c r="D2" s="3">
-        <v>199</v>
+        <v>173</v>
       </c>
       <c r="E2" s="3">
-        <v>69</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -419,16 +419,16 @@
         <v>5</v>
       </c>
       <c r="B3" s="2">
-        <v>2025</v>
+        <v>2022</v>
       </c>
       <c r="C3" s="2">
         <v>2</v>
       </c>
       <c r="D3" s="3">
-        <v>161</v>
+        <v>142</v>
       </c>
       <c r="E3" s="3">
-        <v>48</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -436,16 +436,16 @@
         <v>5</v>
       </c>
       <c r="B4" s="2">
-        <v>2025</v>
+        <v>2022</v>
       </c>
       <c r="C4" s="2">
         <v>3</v>
       </c>
       <c r="D4" s="3">
-        <v>124</v>
+        <v>174</v>
       </c>
       <c r="E4" s="3">
-        <v>37</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -453,16 +453,16 @@
         <v>5</v>
       </c>
       <c r="B5" s="2">
-        <v>2025</v>
+        <v>2022</v>
       </c>
       <c r="C5" s="2">
         <v>4</v>
       </c>
       <c r="D5" s="3">
-        <v>127</v>
+        <v>186</v>
       </c>
       <c r="E5" s="3">
-        <v>49</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -470,16 +470,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="2">
-        <v>2025</v>
+        <v>2022</v>
       </c>
       <c r="C6" s="2">
         <v>5</v>
       </c>
       <c r="D6" s="3">
-        <v>204</v>
+        <v>159</v>
       </c>
       <c r="E6" s="3">
-        <v>77</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -487,16 +487,16 @@
         <v>5</v>
       </c>
       <c r="B7" s="2">
-        <v>2025</v>
+        <v>2022</v>
       </c>
       <c r="C7" s="2">
         <v>6</v>
       </c>
       <c r="D7" s="3">
-        <v>195</v>
+        <v>160</v>
       </c>
       <c r="E7" s="3">
-        <v>65</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -504,16 +504,16 @@
         <v>5</v>
       </c>
       <c r="B8" s="2">
-        <v>2025</v>
+        <v>2022</v>
       </c>
       <c r="C8" s="2">
         <v>7</v>
       </c>
       <c r="D8" s="3">
-        <v>211</v>
+        <v>148</v>
       </c>
       <c r="E8" s="3">
-        <v>84</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -521,16 +521,16 @@
         <v>5</v>
       </c>
       <c r="B9" s="2">
-        <v>2025</v>
+        <v>2022</v>
       </c>
       <c r="C9" s="2">
         <v>8</v>
       </c>
       <c r="D9" s="3">
-        <v>170</v>
+        <v>158</v>
       </c>
       <c r="E9" s="3">
-        <v>78</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -538,16 +538,16 @@
         <v>5</v>
       </c>
       <c r="B10" s="2">
-        <v>2025</v>
+        <v>2022</v>
       </c>
       <c r="C10" s="2">
         <v>9</v>
       </c>
       <c r="D10" s="3">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="E10" s="3">
-        <v>58</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -555,16 +555,16 @@
         <v>5</v>
       </c>
       <c r="B11" s="2">
-        <v>2025</v>
+        <v>2022</v>
       </c>
       <c r="C11" s="2">
         <v>10</v>
       </c>
       <c r="D11" s="3">
-        <v>176</v>
+        <v>137</v>
       </c>
       <c r="E11" s="3">
-        <v>71</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -572,577 +572,3093 @@
         <v>5</v>
       </c>
       <c r="B12" s="2">
-        <v>2025</v>
+        <v>2022</v>
       </c>
       <c r="C12" s="2">
         <v>11</v>
       </c>
       <c r="D12" s="3">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="E12" s="3">
-        <v>45</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B13" s="2">
-        <v>2025</v>
+        <v>2022</v>
       </c>
       <c r="C13" s="2">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="D13" s="3">
-        <v>103</v>
+        <v>164</v>
       </c>
       <c r="E13" s="3">
-        <v>60</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B14" s="2">
-        <v>2025</v>
+        <v>2023</v>
       </c>
       <c r="C14" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D14" s="3">
-        <v>115</v>
+        <v>126</v>
       </c>
       <c r="E14" s="3">
-        <v>63</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B15" s="2">
-        <v>2025</v>
+        <v>2023</v>
       </c>
       <c r="C15" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D15" s="3">
-        <v>113</v>
+        <v>142</v>
       </c>
       <c r="E15" s="3">
-        <v>65</v>
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B16" s="2">
-        <v>2025</v>
+        <v>2023</v>
       </c>
       <c r="C16" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D16" s="3">
-        <v>118</v>
+        <v>159</v>
       </c>
       <c r="E16" s="3">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B17" s="2">
-        <v>2025</v>
+        <v>2023</v>
       </c>
       <c r="C17" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D17" s="3">
-        <v>106</v>
+        <v>148</v>
       </c>
       <c r="E17" s="3">
-        <v>65</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B18" s="2">
-        <v>2025</v>
+        <v>2023</v>
       </c>
       <c r="C18" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D18" s="3">
-        <v>106</v>
+        <v>166</v>
       </c>
       <c r="E18" s="3">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B19" s="2">
-        <v>2025</v>
+        <v>2023</v>
       </c>
       <c r="C19" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D19" s="3">
-        <v>109</v>
+        <v>159</v>
       </c>
       <c r="E19" s="3">
-        <v>64</v>
+        <v>57</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B20" s="2">
-        <v>2025</v>
+        <v>2023</v>
       </c>
       <c r="C20" s="2">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D20" s="3">
-        <v>124</v>
+        <v>162</v>
       </c>
       <c r="E20" s="3">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B21" s="2">
-        <v>2025</v>
+        <v>2023</v>
       </c>
       <c r="C21" s="2">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D21" s="3">
-        <v>126</v>
+        <v>174</v>
       </c>
       <c r="E21" s="3">
-        <v>60</v>
+        <v>72</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B22" s="2">
-        <v>2025</v>
+        <v>2023</v>
       </c>
       <c r="C22" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D22" s="3">
-        <v>106</v>
+        <v>168</v>
       </c>
       <c r="E22" s="3">
-        <v>59</v>
+        <v>74</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B23" s="2">
-        <v>2025</v>
+        <v>2023</v>
       </c>
       <c r="C23" s="2">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D23" s="3">
-        <v>115</v>
+        <v>125</v>
       </c>
       <c r="E23" s="3">
-        <v>54</v>
+        <v>39</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B24" s="2">
-        <v>2025</v>
+        <v>2023</v>
       </c>
       <c r="C24" s="2">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D24" s="3">
-        <v>113</v>
+        <v>161</v>
       </c>
       <c r="E24" s="3">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B25" s="2">
-        <v>2025</v>
+        <v>2023</v>
       </c>
       <c r="C25" s="2">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D25" s="3">
-        <v>110</v>
+        <v>137</v>
       </c>
       <c r="E25" s="3">
-        <v>53</v>
+        <v>44</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B26" s="2">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="C26" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D26" s="3">
-        <v>160</v>
+        <v>179</v>
       </c>
       <c r="E26" s="3">
-        <v>79</v>
+        <v>66</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B27" s="2">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="C27" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D27" s="3">
-        <v>135</v>
+        <v>173</v>
       </c>
       <c r="E27" s="3">
-        <v>56</v>
+        <v>66</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B28" s="2">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="C28" s="2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D28" s="3">
-        <v>139</v>
+        <v>175</v>
       </c>
       <c r="E28" s="3">
-        <v>71</v>
+        <v>57</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B29" s="2">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="C29" s="2">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D29" s="3">
-        <v>127</v>
+        <v>158</v>
       </c>
       <c r="E29" s="3">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B30" s="2">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="C30" s="2">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D30" s="3">
-        <v>131</v>
+        <v>168</v>
       </c>
       <c r="E30" s="3">
-        <v>69</v>
+        <v>75</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B31" s="2">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="C31" s="2">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D31" s="3">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="E31" s="3">
-        <v>67</v>
+        <v>45</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B32" s="2">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="C32" s="2">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D32" s="3">
-        <v>108</v>
+        <v>173</v>
       </c>
       <c r="E32" s="3">
-        <v>54</v>
+        <v>68</v>
       </c>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B33" s="2">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="C33" s="2">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D33" s="3">
-        <v>123</v>
+        <v>169</v>
       </c>
       <c r="E33" s="3">
-        <v>59</v>
+        <v>69</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B34" s="2">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="C34" s="2">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D34" s="3">
-        <v>122</v>
+        <v>150</v>
       </c>
       <c r="E34" s="3">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B35" s="2">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="C35" s="2">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D35" s="3">
-        <v>278</v>
+        <v>155</v>
       </c>
       <c r="E35" s="3">
-        <v>104</v>
+        <v>56</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B36" s="2">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="C36" s="2">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="D36" s="3">
-        <v>242</v>
+        <v>147</v>
       </c>
       <c r="E36" s="3">
-        <v>90</v>
+        <v>50</v>
       </c>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B37" s="2">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="C37" s="2">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="D37" s="3">
-        <v>296</v>
+        <v>175</v>
       </c>
       <c r="E37" s="3">
-        <v>113</v>
+        <v>76</v>
       </c>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B38" s="2">
         <v>2025</v>
       </c>
       <c r="C38" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D38" s="3">
-        <v>296</v>
+        <v>199</v>
       </c>
       <c r="E38" s="3">
-        <v>113</v>
+        <v>69</v>
       </c>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B39" s="2">
         <v>2025</v>
       </c>
       <c r="C39" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D39" s="3">
-        <v>296</v>
+        <v>161</v>
       </c>
       <c r="E39" s="3">
-        <v>119</v>
+        <v>48</v>
       </c>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B40" s="2">
         <v>2025</v>
       </c>
       <c r="C40" s="2">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D40" s="3">
-        <v>286</v>
+        <v>124</v>
       </c>
       <c r="E40" s="3">
-        <v>99</v>
+        <v>37</v>
       </c>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B41" s="2">
         <v>2025</v>
       </c>
       <c r="C41" s="2">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D41" s="3">
-        <v>255</v>
+        <v>127</v>
       </c>
       <c r="E41" s="3">
-        <v>92</v>
+        <v>49</v>
       </c>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B42" s="2">
         <v>2025</v>
       </c>
       <c r="C42" s="2">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D42" s="3">
-        <v>262</v>
+        <v>204</v>
       </c>
       <c r="E42" s="3">
-        <v>97</v>
+        <v>77</v>
       </c>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B43" s="2">
         <v>2025</v>
       </c>
       <c r="C43" s="2">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D43" s="3">
-        <v>248</v>
+        <v>195</v>
       </c>
       <c r="E43" s="3">
-        <v>91</v>
+        <v>65</v>
       </c>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B44" s="2">
         <v>2025</v>
       </c>
       <c r="C44" s="2">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D44" s="3">
-        <v>266</v>
+        <v>211</v>
       </c>
       <c r="E44" s="3">
-        <v>92</v>
+        <v>84</v>
       </c>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B45" s="2">
         <v>2025</v>
       </c>
       <c r="C45" s="2">
+        <v>8</v>
+      </c>
+      <c r="D45" s="3">
+        <v>170</v>
+      </c>
+      <c r="E45" s="3">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" t="s">
+        <v>5</v>
+      </c>
+      <c r="B46" s="2">
+        <v>2025</v>
+      </c>
+      <c r="C46" s="2">
+        <v>9</v>
+      </c>
+      <c r="D46" s="3">
+        <v>176</v>
+      </c>
+      <c r="E46" s="3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" t="s">
+        <v>5</v>
+      </c>
+      <c r="B47" s="2">
+        <v>2025</v>
+      </c>
+      <c r="C47" s="2">
+        <v>10</v>
+      </c>
+      <c r="D47" s="3">
+        <v>176</v>
+      </c>
+      <c r="E47" s="3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" t="s">
+        <v>5</v>
+      </c>
+      <c r="B48" s="2">
+        <v>2025</v>
+      </c>
+      <c r="C48" s="2">
         <v>11</v>
       </c>
-      <c r="D45" s="3">
+      <c r="D48" s="3">
+        <v>137</v>
+      </c>
+      <c r="E48" s="3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" t="s">
+        <v>5</v>
+      </c>
+      <c r="B49" s="2">
+        <v>2025</v>
+      </c>
+      <c r="C49" s="2">
+        <v>12</v>
+      </c>
+      <c r="D49" s="3">
+        <v>162</v>
+      </c>
+      <c r="E49" s="3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" t="s">
+        <v>6</v>
+      </c>
+      <c r="B50" s="2">
+        <v>2022</v>
+      </c>
+      <c r="C50" s="2">
+        <v>1</v>
+      </c>
+      <c r="D50" s="3">
+        <v>115</v>
+      </c>
+      <c r="E50" s="3">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" t="s">
+        <v>6</v>
+      </c>
+      <c r="B51" s="2">
+        <v>2022</v>
+      </c>
+      <c r="C51" s="2">
+        <v>2</v>
+      </c>
+      <c r="D51" s="3">
+        <v>120</v>
+      </c>
+      <c r="E51" s="3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" t="s">
+        <v>6</v>
+      </c>
+      <c r="B52" s="2">
+        <v>2022</v>
+      </c>
+      <c r="C52" s="2">
+        <v>3</v>
+      </c>
+      <c r="D52" s="3">
+        <v>126</v>
+      </c>
+      <c r="E52" s="3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" t="s">
+        <v>6</v>
+      </c>
+      <c r="B53" s="2">
+        <v>2022</v>
+      </c>
+      <c r="C53" s="2">
+        <v>4</v>
+      </c>
+      <c r="D53" s="3">
+        <v>109</v>
+      </c>
+      <c r="E53" s="3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" t="s">
+        <v>6</v>
+      </c>
+      <c r="B54" s="2">
+        <v>2022</v>
+      </c>
+      <c r="C54" s="2">
+        <v>5</v>
+      </c>
+      <c r="D54" s="3">
+        <v>107</v>
+      </c>
+      <c r="E54" s="3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" t="s">
+        <v>6</v>
+      </c>
+      <c r="B55" s="2">
+        <v>2022</v>
+      </c>
+      <c r="C55" s="2">
+        <v>6</v>
+      </c>
+      <c r="D55" s="3">
+        <v>99</v>
+      </c>
+      <c r="E55" s="3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56" t="s">
+        <v>6</v>
+      </c>
+      <c r="B56" s="2">
+        <v>2022</v>
+      </c>
+      <c r="C56" s="2">
+        <v>7</v>
+      </c>
+      <c r="D56" s="3">
+        <v>84</v>
+      </c>
+      <c r="E56" s="3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57" t="s">
+        <v>6</v>
+      </c>
+      <c r="B57" s="2">
+        <v>2022</v>
+      </c>
+      <c r="C57" s="2">
+        <v>8</v>
+      </c>
+      <c r="D57" s="3">
+        <v>119</v>
+      </c>
+      <c r="E57" s="3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58" t="s">
+        <v>6</v>
+      </c>
+      <c r="B58" s="2">
+        <v>2022</v>
+      </c>
+      <c r="C58" s="2">
+        <v>9</v>
+      </c>
+      <c r="D58" s="3">
+        <v>82</v>
+      </c>
+      <c r="E58" s="3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59" t="s">
+        <v>6</v>
+      </c>
+      <c r="B59" s="2">
+        <v>2022</v>
+      </c>
+      <c r="C59" s="2">
+        <v>10</v>
+      </c>
+      <c r="D59" s="3">
+        <v>96</v>
+      </c>
+      <c r="E59" s="3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60" t="s">
+        <v>6</v>
+      </c>
+      <c r="B60" s="2">
+        <v>2022</v>
+      </c>
+      <c r="C60" s="2">
+        <v>11</v>
+      </c>
+      <c r="D60" s="3">
+        <v>118</v>
+      </c>
+      <c r="E60" s="3">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61" t="s">
+        <v>6</v>
+      </c>
+      <c r="B61" s="2">
+        <v>2022</v>
+      </c>
+      <c r="C61" s="2">
+        <v>12</v>
+      </c>
+      <c r="D61" s="3">
+        <v>104</v>
+      </c>
+      <c r="E61" s="3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62" t="s">
+        <v>6</v>
+      </c>
+      <c r="B62" s="2">
+        <v>2023</v>
+      </c>
+      <c r="C62" s="2">
+        <v>1</v>
+      </c>
+      <c r="D62" s="3">
+        <v>129</v>
+      </c>
+      <c r="E62" s="3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63" t="s">
+        <v>6</v>
+      </c>
+      <c r="B63" s="2">
+        <v>2023</v>
+      </c>
+      <c r="C63" s="2">
+        <v>2</v>
+      </c>
+      <c r="D63" s="3">
+        <v>101</v>
+      </c>
+      <c r="E63" s="3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64" t="s">
+        <v>6</v>
+      </c>
+      <c r="B64" s="2">
+        <v>2023</v>
+      </c>
+      <c r="C64" s="2">
+        <v>3</v>
+      </c>
+      <c r="D64" s="3">
+        <v>115</v>
+      </c>
+      <c r="E64" s="3">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
+      <c r="A65" t="s">
+        <v>6</v>
+      </c>
+      <c r="B65" s="2">
+        <v>2023</v>
+      </c>
+      <c r="C65" s="2">
+        <v>4</v>
+      </c>
+      <c r="D65" s="3">
+        <v>119</v>
+      </c>
+      <c r="E65" s="3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5">
+      <c r="A66" t="s">
+        <v>6</v>
+      </c>
+      <c r="B66" s="2">
+        <v>2023</v>
+      </c>
+      <c r="C66" s="2">
+        <v>5</v>
+      </c>
+      <c r="D66" s="3">
+        <v>103</v>
+      </c>
+      <c r="E66" s="3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
+      <c r="A67" t="s">
+        <v>6</v>
+      </c>
+      <c r="B67" s="2">
+        <v>2023</v>
+      </c>
+      <c r="C67" s="2">
+        <v>6</v>
+      </c>
+      <c r="D67" s="3">
+        <v>121</v>
+      </c>
+      <c r="E67" s="3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5">
+      <c r="A68" t="s">
+        <v>6</v>
+      </c>
+      <c r="B68" s="2">
+        <v>2023</v>
+      </c>
+      <c r="C68" s="2">
+        <v>7</v>
+      </c>
+      <c r="D68" s="3">
+        <v>99</v>
+      </c>
+      <c r="E68" s="3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5">
+      <c r="A69" t="s">
+        <v>6</v>
+      </c>
+      <c r="B69" s="2">
+        <v>2023</v>
+      </c>
+      <c r="C69" s="2">
+        <v>8</v>
+      </c>
+      <c r="D69" s="3">
+        <v>110</v>
+      </c>
+      <c r="E69" s="3">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5">
+      <c r="A70" t="s">
+        <v>6</v>
+      </c>
+      <c r="B70" s="2">
+        <v>2023</v>
+      </c>
+      <c r="C70" s="2">
+        <v>9</v>
+      </c>
+      <c r="D70" s="3">
+        <v>126</v>
+      </c>
+      <c r="E70" s="3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5">
+      <c r="A71" t="s">
+        <v>6</v>
+      </c>
+      <c r="B71" s="2">
+        <v>2023</v>
+      </c>
+      <c r="C71" s="2">
+        <v>10</v>
+      </c>
+      <c r="D71" s="3">
+        <v>98</v>
+      </c>
+      <c r="E71" s="3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5">
+      <c r="A72" t="s">
+        <v>6</v>
+      </c>
+      <c r="B72" s="2">
+        <v>2023</v>
+      </c>
+      <c r="C72" s="2">
+        <v>11</v>
+      </c>
+      <c r="D72" s="3">
+        <v>137</v>
+      </c>
+      <c r="E72" s="3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5">
+      <c r="A73" t="s">
+        <v>6</v>
+      </c>
+      <c r="B73" s="2">
+        <v>2023</v>
+      </c>
+      <c r="C73" s="2">
+        <v>12</v>
+      </c>
+      <c r="D73" s="3">
+        <v>96</v>
+      </c>
+      <c r="E73" s="3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5">
+      <c r="A74" t="s">
+        <v>6</v>
+      </c>
+      <c r="B74" s="2">
+        <v>2024</v>
+      </c>
+      <c r="C74" s="2">
+        <v>1</v>
+      </c>
+      <c r="D74" s="3">
+        <v>112</v>
+      </c>
+      <c r="E74" s="3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5">
+      <c r="A75" t="s">
+        <v>6</v>
+      </c>
+      <c r="B75" s="2">
+        <v>2024</v>
+      </c>
+      <c r="C75" s="2">
+        <v>2</v>
+      </c>
+      <c r="D75" s="3">
+        <v>97</v>
+      </c>
+      <c r="E75" s="3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5">
+      <c r="A76" t="s">
+        <v>6</v>
+      </c>
+      <c r="B76" s="2">
+        <v>2024</v>
+      </c>
+      <c r="C76" s="2">
+        <v>3</v>
+      </c>
+      <c r="D76" s="3">
+        <v>113</v>
+      </c>
+      <c r="E76" s="3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5">
+      <c r="A77" t="s">
+        <v>6</v>
+      </c>
+      <c r="B77" s="2">
+        <v>2024</v>
+      </c>
+      <c r="C77" s="2">
+        <v>4</v>
+      </c>
+      <c r="D77" s="3">
+        <v>98</v>
+      </c>
+      <c r="E77" s="3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5">
+      <c r="A78" t="s">
+        <v>6</v>
+      </c>
+      <c r="B78" s="2">
+        <v>2024</v>
+      </c>
+      <c r="C78" s="2">
+        <v>5</v>
+      </c>
+      <c r="D78" s="3">
+        <v>116</v>
+      </c>
+      <c r="E78" s="3">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5">
+      <c r="A79" t="s">
+        <v>6</v>
+      </c>
+      <c r="B79" s="2">
+        <v>2024</v>
+      </c>
+      <c r="C79" s="2">
+        <v>6</v>
+      </c>
+      <c r="D79" s="3">
+        <v>107</v>
+      </c>
+      <c r="E79" s="3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5">
+      <c r="A80" t="s">
+        <v>6</v>
+      </c>
+      <c r="B80" s="2">
+        <v>2024</v>
+      </c>
+      <c r="C80" s="2">
+        <v>7</v>
+      </c>
+      <c r="D80" s="3">
+        <v>80</v>
+      </c>
+      <c r="E80" s="3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5">
+      <c r="A81" t="s">
+        <v>6</v>
+      </c>
+      <c r="B81" s="2">
+        <v>2024</v>
+      </c>
+      <c r="C81" s="2">
+        <v>8</v>
+      </c>
+      <c r="D81" s="3">
+        <v>92</v>
+      </c>
+      <c r="E81" s="3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5">
+      <c r="A82" t="s">
+        <v>6</v>
+      </c>
+      <c r="B82" s="2">
+        <v>2024</v>
+      </c>
+      <c r="C82" s="2">
+        <v>9</v>
+      </c>
+      <c r="D82" s="3">
+        <v>113</v>
+      </c>
+      <c r="E82" s="3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5">
+      <c r="A83" t="s">
+        <v>6</v>
+      </c>
+      <c r="B83" s="2">
+        <v>2024</v>
+      </c>
+      <c r="C83" s="2">
+        <v>10</v>
+      </c>
+      <c r="D83" s="3">
+        <v>100</v>
+      </c>
+      <c r="E83" s="3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5">
+      <c r="A84" t="s">
+        <v>6</v>
+      </c>
+      <c r="B84" s="2">
+        <v>2024</v>
+      </c>
+      <c r="C84" s="2">
+        <v>11</v>
+      </c>
+      <c r="D84" s="3">
+        <v>90</v>
+      </c>
+      <c r="E84" s="3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5">
+      <c r="A85" t="s">
+        <v>6</v>
+      </c>
+      <c r="B85" s="2">
+        <v>2024</v>
+      </c>
+      <c r="C85" s="2">
+        <v>12</v>
+      </c>
+      <c r="D85" s="3">
+        <v>126</v>
+      </c>
+      <c r="E85" s="3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5">
+      <c r="A86" t="s">
+        <v>6</v>
+      </c>
+      <c r="B86" s="2">
+        <v>2025</v>
+      </c>
+      <c r="C86" s="2">
+        <v>1</v>
+      </c>
+      <c r="D86" s="3">
+        <v>103</v>
+      </c>
+      <c r="E86" s="3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5">
+      <c r="A87" t="s">
+        <v>6</v>
+      </c>
+      <c r="B87" s="2">
+        <v>2025</v>
+      </c>
+      <c r="C87" s="2">
+        <v>2</v>
+      </c>
+      <c r="D87" s="3">
+        <v>115</v>
+      </c>
+      <c r="E87" s="3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5">
+      <c r="A88" t="s">
+        <v>6</v>
+      </c>
+      <c r="B88" s="2">
+        <v>2025</v>
+      </c>
+      <c r="C88" s="2">
+        <v>3</v>
+      </c>
+      <c r="D88" s="3">
+        <v>113</v>
+      </c>
+      <c r="E88" s="3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5">
+      <c r="A89" t="s">
+        <v>6</v>
+      </c>
+      <c r="B89" s="2">
+        <v>2025</v>
+      </c>
+      <c r="C89" s="2">
+        <v>4</v>
+      </c>
+      <c r="D89" s="3">
+        <v>118</v>
+      </c>
+      <c r="E89" s="3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5">
+      <c r="A90" t="s">
+        <v>6</v>
+      </c>
+      <c r="B90" s="2">
+        <v>2025</v>
+      </c>
+      <c r="C90" s="2">
+        <v>5</v>
+      </c>
+      <c r="D90" s="3">
+        <v>106</v>
+      </c>
+      <c r="E90" s="3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5">
+      <c r="A91" t="s">
+        <v>6</v>
+      </c>
+      <c r="B91" s="2">
+        <v>2025</v>
+      </c>
+      <c r="C91" s="2">
+        <v>6</v>
+      </c>
+      <c r="D91" s="3">
+        <v>106</v>
+      </c>
+      <c r="E91" s="3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5">
+      <c r="A92" t="s">
+        <v>6</v>
+      </c>
+      <c r="B92" s="2">
+        <v>2025</v>
+      </c>
+      <c r="C92" s="2">
+        <v>7</v>
+      </c>
+      <c r="D92" s="3">
+        <v>109</v>
+      </c>
+      <c r="E92" s="3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5">
+      <c r="A93" t="s">
+        <v>6</v>
+      </c>
+      <c r="B93" s="2">
+        <v>2025</v>
+      </c>
+      <c r="C93" s="2">
+        <v>8</v>
+      </c>
+      <c r="D93" s="3">
+        <v>124</v>
+      </c>
+      <c r="E93" s="3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5">
+      <c r="A94" t="s">
+        <v>6</v>
+      </c>
+      <c r="B94" s="2">
+        <v>2025</v>
+      </c>
+      <c r="C94" s="2">
+        <v>9</v>
+      </c>
+      <c r="D94" s="3">
+        <v>126</v>
+      </c>
+      <c r="E94" s="3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5">
+      <c r="A95" t="s">
+        <v>6</v>
+      </c>
+      <c r="B95" s="2">
+        <v>2025</v>
+      </c>
+      <c r="C95" s="2">
+        <v>10</v>
+      </c>
+      <c r="D95" s="3">
+        <v>106</v>
+      </c>
+      <c r="E95" s="3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5">
+      <c r="A96" t="s">
+        <v>6</v>
+      </c>
+      <c r="B96" s="2">
+        <v>2025</v>
+      </c>
+      <c r="C96" s="2">
+        <v>11</v>
+      </c>
+      <c r="D96" s="3">
+        <v>115</v>
+      </c>
+      <c r="E96" s="3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5">
+      <c r="A97" t="s">
+        <v>6</v>
+      </c>
+      <c r="B97" s="2">
+        <v>2025</v>
+      </c>
+      <c r="C97" s="2">
+        <v>12</v>
+      </c>
+      <c r="D97" s="3">
+        <v>95</v>
+      </c>
+      <c r="E97" s="3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5">
+      <c r="A98" t="s">
+        <v>7</v>
+      </c>
+      <c r="B98" s="2">
+        <v>2022</v>
+      </c>
+      <c r="C98" s="2">
+        <v>1</v>
+      </c>
+      <c r="D98" s="3">
+        <v>124</v>
+      </c>
+      <c r="E98" s="3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5">
+      <c r="A99" t="s">
+        <v>7</v>
+      </c>
+      <c r="B99" s="2">
+        <v>2022</v>
+      </c>
+      <c r="C99" s="2">
+        <v>2</v>
+      </c>
+      <c r="D99" s="3">
+        <v>110</v>
+      </c>
+      <c r="E99" s="3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5">
+      <c r="A100" t="s">
+        <v>7</v>
+      </c>
+      <c r="B100" s="2">
+        <v>2022</v>
+      </c>
+      <c r="C100" s="2">
+        <v>3</v>
+      </c>
+      <c r="D100" s="3">
+        <v>116</v>
+      </c>
+      <c r="E100" s="3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5">
+      <c r="A101" t="s">
+        <v>7</v>
+      </c>
+      <c r="B101" s="2">
+        <v>2022</v>
+      </c>
+      <c r="C101" s="2">
+        <v>4</v>
+      </c>
+      <c r="D101" s="3">
+        <v>128</v>
+      </c>
+      <c r="E101" s="3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5">
+      <c r="A102" t="s">
+        <v>7</v>
+      </c>
+      <c r="B102" s="2">
+        <v>2022</v>
+      </c>
+      <c r="C102" s="2">
+        <v>5</v>
+      </c>
+      <c r="D102" s="3">
+        <v>119</v>
+      </c>
+      <c r="E102" s="3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5">
+      <c r="A103" t="s">
+        <v>7</v>
+      </c>
+      <c r="B103" s="2">
+        <v>2022</v>
+      </c>
+      <c r="C103" s="2">
+        <v>6</v>
+      </c>
+      <c r="D103" s="3">
+        <v>108</v>
+      </c>
+      <c r="E103" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5">
+      <c r="A104" t="s">
+        <v>7</v>
+      </c>
+      <c r="B104" s="2">
+        <v>2022</v>
+      </c>
+      <c r="C104" s="2">
+        <v>7</v>
+      </c>
+      <c r="D104" s="3">
+        <v>118</v>
+      </c>
+      <c r="E104" s="3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5">
+      <c r="A105" t="s">
+        <v>7</v>
+      </c>
+      <c r="B105" s="2">
+        <v>2022</v>
+      </c>
+      <c r="C105" s="2">
+        <v>8</v>
+      </c>
+      <c r="D105" s="3">
+        <v>99</v>
+      </c>
+      <c r="E105" s="3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5">
+      <c r="A106" t="s">
+        <v>7</v>
+      </c>
+      <c r="B106" s="2">
+        <v>2022</v>
+      </c>
+      <c r="C106" s="2">
+        <v>9</v>
+      </c>
+      <c r="D106" s="3">
+        <v>104</v>
+      </c>
+      <c r="E106" s="3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5">
+      <c r="A107" t="s">
+        <v>7</v>
+      </c>
+      <c r="B107" s="2">
+        <v>2022</v>
+      </c>
+      <c r="C107" s="2">
+        <v>10</v>
+      </c>
+      <c r="D107" s="3">
+        <v>83</v>
+      </c>
+      <c r="E107" s="3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5">
+      <c r="A108" t="s">
+        <v>7</v>
+      </c>
+      <c r="B108" s="2">
+        <v>2022</v>
+      </c>
+      <c r="C108" s="2">
+        <v>11</v>
+      </c>
+      <c r="D108" s="3">
+        <v>96</v>
+      </c>
+      <c r="E108" s="3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5">
+      <c r="A109" t="s">
+        <v>7</v>
+      </c>
+      <c r="B109" s="2">
+        <v>2022</v>
+      </c>
+      <c r="C109" s="2">
+        <v>12</v>
+      </c>
+      <c r="D109" s="3">
+        <v>110</v>
+      </c>
+      <c r="E109" s="3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5">
+      <c r="A110" t="s">
+        <v>7</v>
+      </c>
+      <c r="B110" s="2">
+        <v>2023</v>
+      </c>
+      <c r="C110" s="2">
+        <v>1</v>
+      </c>
+      <c r="D110" s="3">
+        <v>109</v>
+      </c>
+      <c r="E110" s="3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5">
+      <c r="A111" t="s">
+        <v>7</v>
+      </c>
+      <c r="B111" s="2">
+        <v>2023</v>
+      </c>
+      <c r="C111" s="2">
+        <v>2</v>
+      </c>
+      <c r="D111" s="3">
+        <v>97</v>
+      </c>
+      <c r="E111" s="3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5">
+      <c r="A112" t="s">
+        <v>7</v>
+      </c>
+      <c r="B112" s="2">
+        <v>2023</v>
+      </c>
+      <c r="C112" s="2">
+        <v>3</v>
+      </c>
+      <c r="D112" s="3">
+        <v>125</v>
+      </c>
+      <c r="E112" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5">
+      <c r="A113" t="s">
+        <v>7</v>
+      </c>
+      <c r="B113" s="2">
+        <v>2023</v>
+      </c>
+      <c r="C113" s="2">
+        <v>4</v>
+      </c>
+      <c r="D113" s="3">
+        <v>118</v>
+      </c>
+      <c r="E113" s="3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5">
+      <c r="A114" t="s">
+        <v>7</v>
+      </c>
+      <c r="B114" s="2">
+        <v>2023</v>
+      </c>
+      <c r="C114" s="2">
+        <v>5</v>
+      </c>
+      <c r="D114" s="3">
+        <v>114</v>
+      </c>
+      <c r="E114" s="3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5">
+      <c r="A115" t="s">
+        <v>7</v>
+      </c>
+      <c r="B115" s="2">
+        <v>2023</v>
+      </c>
+      <c r="C115" s="2">
+        <v>6</v>
+      </c>
+      <c r="D115" s="3">
+        <v>109</v>
+      </c>
+      <c r="E115" s="3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5">
+      <c r="A116" t="s">
+        <v>7</v>
+      </c>
+      <c r="B116" s="2">
+        <v>2023</v>
+      </c>
+      <c r="C116" s="2">
+        <v>7</v>
+      </c>
+      <c r="D116" s="3">
+        <v>110</v>
+      </c>
+      <c r="E116" s="3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5">
+      <c r="A117" t="s">
+        <v>7</v>
+      </c>
+      <c r="B117" s="2">
+        <v>2023</v>
+      </c>
+      <c r="C117" s="2">
+        <v>8</v>
+      </c>
+      <c r="D117" s="3">
+        <v>94</v>
+      </c>
+      <c r="E117" s="3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5">
+      <c r="A118" t="s">
+        <v>7</v>
+      </c>
+      <c r="B118" s="2">
+        <v>2023</v>
+      </c>
+      <c r="C118" s="2">
+        <v>9</v>
+      </c>
+      <c r="D118" s="3">
+        <v>98</v>
+      </c>
+      <c r="E118" s="3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5">
+      <c r="A119" t="s">
+        <v>7</v>
+      </c>
+      <c r="B119" s="2">
+        <v>2023</v>
+      </c>
+      <c r="C119" s="2">
+        <v>10</v>
+      </c>
+      <c r="D119" s="3">
+        <v>109</v>
+      </c>
+      <c r="E119" s="3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5">
+      <c r="A120" t="s">
+        <v>7</v>
+      </c>
+      <c r="B120" s="2">
+        <v>2023</v>
+      </c>
+      <c r="C120" s="2">
+        <v>11</v>
+      </c>
+      <c r="D120" s="3">
+        <v>120</v>
+      </c>
+      <c r="E120" s="3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5">
+      <c r="A121" t="s">
+        <v>7</v>
+      </c>
+      <c r="B121" s="2">
+        <v>2023</v>
+      </c>
+      <c r="C121" s="2">
+        <v>12</v>
+      </c>
+      <c r="D121" s="3">
+        <v>105</v>
+      </c>
+      <c r="E121" s="3">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5">
+      <c r="A122" t="s">
+        <v>7</v>
+      </c>
+      <c r="B122" s="2">
+        <v>2024</v>
+      </c>
+      <c r="C122" s="2">
+        <v>1</v>
+      </c>
+      <c r="D122" s="3">
+        <v>115</v>
+      </c>
+      <c r="E122" s="3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5">
+      <c r="A123" t="s">
+        <v>7</v>
+      </c>
+      <c r="B123" s="2">
+        <v>2024</v>
+      </c>
+      <c r="C123" s="2">
+        <v>2</v>
+      </c>
+      <c r="D123" s="3">
+        <v>99</v>
+      </c>
+      <c r="E123" s="3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5">
+      <c r="A124" t="s">
+        <v>7</v>
+      </c>
+      <c r="B124" s="2">
+        <v>2024</v>
+      </c>
+      <c r="C124" s="2">
+        <v>3</v>
+      </c>
+      <c r="D124" s="3">
+        <v>99</v>
+      </c>
+      <c r="E124" s="3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5">
+      <c r="A125" t="s">
+        <v>7</v>
+      </c>
+      <c r="B125" s="2">
+        <v>2024</v>
+      </c>
+      <c r="C125" s="2">
+        <v>4</v>
+      </c>
+      <c r="D125" s="3">
+        <v>113</v>
+      </c>
+      <c r="E125" s="3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5">
+      <c r="A126" t="s">
+        <v>7</v>
+      </c>
+      <c r="B126" s="2">
+        <v>2024</v>
+      </c>
+      <c r="C126" s="2">
+        <v>5</v>
+      </c>
+      <c r="D126" s="3">
+        <v>117</v>
+      </c>
+      <c r="E126" s="3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5">
+      <c r="A127" t="s">
+        <v>7</v>
+      </c>
+      <c r="B127" s="2">
+        <v>2024</v>
+      </c>
+      <c r="C127" s="2">
+        <v>6</v>
+      </c>
+      <c r="D127" s="3">
+        <v>124</v>
+      </c>
+      <c r="E127" s="3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5">
+      <c r="A128" t="s">
+        <v>7</v>
+      </c>
+      <c r="B128" s="2">
+        <v>2024</v>
+      </c>
+      <c r="C128" s="2">
+        <v>7</v>
+      </c>
+      <c r="D128" s="3">
+        <v>102</v>
+      </c>
+      <c r="E128" s="3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5">
+      <c r="A129" t="s">
+        <v>7</v>
+      </c>
+      <c r="B129" s="2">
+        <v>2024</v>
+      </c>
+      <c r="C129" s="2">
+        <v>8</v>
+      </c>
+      <c r="D129" s="3">
+        <v>101</v>
+      </c>
+      <c r="E129" s="3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5">
+      <c r="A130" t="s">
+        <v>7</v>
+      </c>
+      <c r="B130" s="2">
+        <v>2024</v>
+      </c>
+      <c r="C130" s="2">
+        <v>9</v>
+      </c>
+      <c r="D130" s="3">
+        <v>120</v>
+      </c>
+      <c r="E130" s="3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5">
+      <c r="A131" t="s">
+        <v>7</v>
+      </c>
+      <c r="B131" s="2">
+        <v>2024</v>
+      </c>
+      <c r="C131" s="2">
+        <v>10</v>
+      </c>
+      <c r="D131" s="3">
+        <v>118</v>
+      </c>
+      <c r="E131" s="3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5">
+      <c r="A132" t="s">
+        <v>7</v>
+      </c>
+      <c r="B132" s="2">
+        <v>2024</v>
+      </c>
+      <c r="C132" s="2">
+        <v>11</v>
+      </c>
+      <c r="D132" s="3">
+        <v>89</v>
+      </c>
+      <c r="E132" s="3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5">
+      <c r="A133" t="s">
+        <v>7</v>
+      </c>
+      <c r="B133" s="2">
+        <v>2024</v>
+      </c>
+      <c r="C133" s="2">
+        <v>12</v>
+      </c>
+      <c r="D133" s="3">
+        <v>99</v>
+      </c>
+      <c r="E133" s="3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5">
+      <c r="A134" t="s">
+        <v>7</v>
+      </c>
+      <c r="B134" s="2">
+        <v>2025</v>
+      </c>
+      <c r="C134" s="2">
+        <v>1</v>
+      </c>
+      <c r="D134" s="3">
+        <v>113</v>
+      </c>
+      <c r="E134" s="3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5">
+      <c r="A135" t="s">
+        <v>7</v>
+      </c>
+      <c r="B135" s="2">
+        <v>2025</v>
+      </c>
+      <c r="C135" s="2">
+        <v>2</v>
+      </c>
+      <c r="D135" s="3">
+        <v>110</v>
+      </c>
+      <c r="E135" s="3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5">
+      <c r="A136" t="s">
+        <v>7</v>
+      </c>
+      <c r="B136" s="2">
+        <v>2025</v>
+      </c>
+      <c r="C136" s="2">
+        <v>3</v>
+      </c>
+      <c r="D136" s="3">
+        <v>160</v>
+      </c>
+      <c r="E136" s="3">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5">
+      <c r="A137" t="s">
+        <v>7</v>
+      </c>
+      <c r="B137" s="2">
+        <v>2025</v>
+      </c>
+      <c r="C137" s="2">
+        <v>4</v>
+      </c>
+      <c r="D137" s="3">
+        <v>135</v>
+      </c>
+      <c r="E137" s="3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5">
+      <c r="A138" t="s">
+        <v>7</v>
+      </c>
+      <c r="B138" s="2">
+        <v>2025</v>
+      </c>
+      <c r="C138" s="2">
+        <v>5</v>
+      </c>
+      <c r="D138" s="3">
+        <v>139</v>
+      </c>
+      <c r="E138" s="3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5">
+      <c r="A139" t="s">
+        <v>7</v>
+      </c>
+      <c r="B139" s="2">
+        <v>2025</v>
+      </c>
+      <c r="C139" s="2">
+        <v>6</v>
+      </c>
+      <c r="D139" s="3">
+        <v>127</v>
+      </c>
+      <c r="E139" s="3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5">
+      <c r="A140" t="s">
+        <v>7</v>
+      </c>
+      <c r="B140" s="2">
+        <v>2025</v>
+      </c>
+      <c r="C140" s="2">
+        <v>7</v>
+      </c>
+      <c r="D140" s="3">
+        <v>131</v>
+      </c>
+      <c r="E140" s="3">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5">
+      <c r="A141" t="s">
+        <v>7</v>
+      </c>
+      <c r="B141" s="2">
+        <v>2025</v>
+      </c>
+      <c r="C141" s="2">
+        <v>8</v>
+      </c>
+      <c r="D141" s="3">
+        <v>139</v>
+      </c>
+      <c r="E141" s="3">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5">
+      <c r="A142" t="s">
+        <v>7</v>
+      </c>
+      <c r="B142" s="2">
+        <v>2025</v>
+      </c>
+      <c r="C142" s="2">
+        <v>9</v>
+      </c>
+      <c r="D142" s="3">
+        <v>108</v>
+      </c>
+      <c r="E142" s="3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5">
+      <c r="A143" t="s">
+        <v>7</v>
+      </c>
+      <c r="B143" s="2">
+        <v>2025</v>
+      </c>
+      <c r="C143" s="2">
+        <v>10</v>
+      </c>
+      <c r="D143" s="3">
+        <v>123</v>
+      </c>
+      <c r="E143" s="3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5">
+      <c r="A144" t="s">
+        <v>7</v>
+      </c>
+      <c r="B144" s="2">
+        <v>2025</v>
+      </c>
+      <c r="C144" s="2">
+        <v>11</v>
+      </c>
+      <c r="D144" s="3">
+        <v>122</v>
+      </c>
+      <c r="E144" s="3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5">
+      <c r="A145" t="s">
+        <v>7</v>
+      </c>
+      <c r="B145" s="2">
+        <v>2025</v>
+      </c>
+      <c r="C145" s="2">
+        <v>12</v>
+      </c>
+      <c r="D145" s="3">
+        <v>114</v>
+      </c>
+      <c r="E145" s="3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5">
+      <c r="A146" t="s">
+        <v>8</v>
+      </c>
+      <c r="B146" s="2">
+        <v>2022</v>
+      </c>
+      <c r="C146" s="2">
+        <v>1</v>
+      </c>
+      <c r="D146" s="3">
+        <v>245</v>
+      </c>
+      <c r="E146" s="3">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5">
+      <c r="A147" t="s">
+        <v>8</v>
+      </c>
+      <c r="B147" s="2">
+        <v>2022</v>
+      </c>
+      <c r="C147" s="2">
+        <v>2</v>
+      </c>
+      <c r="D147" s="3">
+        <v>224</v>
+      </c>
+      <c r="E147" s="3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5">
+      <c r="A148" t="s">
+        <v>8</v>
+      </c>
+      <c r="B148" s="2">
+        <v>2022</v>
+      </c>
+      <c r="C148" s="2">
+        <v>3</v>
+      </c>
+      <c r="D148" s="3">
+        <v>278</v>
+      </c>
+      <c r="E148" s="3">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5">
+      <c r="A149" t="s">
+        <v>8</v>
+      </c>
+      <c r="B149" s="2">
+        <v>2022</v>
+      </c>
+      <c r="C149" s="2">
+        <v>4</v>
+      </c>
+      <c r="D149" s="3">
+        <v>236</v>
+      </c>
+      <c r="E149" s="3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5">
+      <c r="A150" t="s">
+        <v>8</v>
+      </c>
+      <c r="B150" s="2">
+        <v>2022</v>
+      </c>
+      <c r="C150" s="2">
+        <v>5</v>
+      </c>
+      <c r="D150" s="3">
+        <v>277</v>
+      </c>
+      <c r="E150" s="3">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5">
+      <c r="A151" t="s">
+        <v>8</v>
+      </c>
+      <c r="B151" s="2">
+        <v>2022</v>
+      </c>
+      <c r="C151" s="2">
+        <v>6</v>
+      </c>
+      <c r="D151" s="3">
+        <v>253</v>
+      </c>
+      <c r="E151" s="3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5">
+      <c r="A152" t="s">
+        <v>8</v>
+      </c>
+      <c r="B152" s="2">
+        <v>2022</v>
+      </c>
+      <c r="C152" s="2">
+        <v>7</v>
+      </c>
+      <c r="D152" s="3">
+        <v>265</v>
+      </c>
+      <c r="E152" s="3">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5">
+      <c r="A153" t="s">
+        <v>8</v>
+      </c>
+      <c r="B153" s="2">
+        <v>2022</v>
+      </c>
+      <c r="C153" s="2">
+        <v>8</v>
+      </c>
+      <c r="D153" s="3">
+        <v>239</v>
+      </c>
+      <c r="E153" s="3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5">
+      <c r="A154" t="s">
+        <v>8</v>
+      </c>
+      <c r="B154" s="2">
+        <v>2022</v>
+      </c>
+      <c r="C154" s="2">
+        <v>9</v>
+      </c>
+      <c r="D154" s="3">
+        <v>237</v>
+      </c>
+      <c r="E154" s="3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5">
+      <c r="A155" t="s">
+        <v>8</v>
+      </c>
+      <c r="B155" s="2">
+        <v>2022</v>
+      </c>
+      <c r="C155" s="2">
+        <v>10</v>
+      </c>
+      <c r="D155" s="3">
+        <v>236</v>
+      </c>
+      <c r="E155" s="3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5">
+      <c r="A156" t="s">
+        <v>8</v>
+      </c>
+      <c r="B156" s="2">
+        <v>2022</v>
+      </c>
+      <c r="C156" s="2">
+        <v>11</v>
+      </c>
+      <c r="D156" s="3">
+        <v>245</v>
+      </c>
+      <c r="E156" s="3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5">
+      <c r="A157" t="s">
+        <v>8</v>
+      </c>
+      <c r="B157" s="2">
+        <v>2022</v>
+      </c>
+      <c r="C157" s="2">
+        <v>12</v>
+      </c>
+      <c r="D157" s="3">
+        <v>281</v>
+      </c>
+      <c r="E157" s="3">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5">
+      <c r="A158" t="s">
+        <v>8</v>
+      </c>
+      <c r="B158" s="2">
+        <v>2023</v>
+      </c>
+      <c r="C158" s="2">
+        <v>1</v>
+      </c>
+      <c r="D158" s="3">
+        <v>274</v>
+      </c>
+      <c r="E158" s="3">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5">
+      <c r="A159" t="s">
+        <v>8</v>
+      </c>
+      <c r="B159" s="2">
+        <v>2023</v>
+      </c>
+      <c r="C159" s="2">
+        <v>2</v>
+      </c>
+      <c r="D159" s="3">
+        <v>270</v>
+      </c>
+      <c r="E159" s="3">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5">
+      <c r="A160" t="s">
+        <v>8</v>
+      </c>
+      <c r="B160" s="2">
+        <v>2023</v>
+      </c>
+      <c r="C160" s="2">
+        <v>3</v>
+      </c>
+      <c r="D160" s="3">
+        <v>314</v>
+      </c>
+      <c r="E160" s="3">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5">
+      <c r="A161" t="s">
+        <v>8</v>
+      </c>
+      <c r="B161" s="2">
+        <v>2023</v>
+      </c>
+      <c r="C161" s="2">
+        <v>4</v>
+      </c>
+      <c r="D161" s="3">
+        <v>508</v>
+      </c>
+      <c r="E161" s="3">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5">
+      <c r="A162" t="s">
+        <v>8</v>
+      </c>
+      <c r="B162" s="2">
+        <v>2023</v>
+      </c>
+      <c r="C162" s="2">
+        <v>5</v>
+      </c>
+      <c r="D162" s="3">
+        <v>269</v>
+      </c>
+      <c r="E162" s="3">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5">
+      <c r="A163" t="s">
+        <v>8</v>
+      </c>
+      <c r="B163" s="2">
+        <v>2023</v>
+      </c>
+      <c r="C163" s="2">
+        <v>6</v>
+      </c>
+      <c r="D163" s="3">
+        <v>274</v>
+      </c>
+      <c r="E163" s="3">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5">
+      <c r="A164" t="s">
+        <v>8</v>
+      </c>
+      <c r="B164" s="2">
+        <v>2023</v>
+      </c>
+      <c r="C164" s="2">
+        <v>7</v>
+      </c>
+      <c r="D164" s="3">
+        <v>257</v>
+      </c>
+      <c r="E164" s="3">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5">
+      <c r="A165" t="s">
+        <v>8</v>
+      </c>
+      <c r="B165" s="2">
+        <v>2023</v>
+      </c>
+      <c r="C165" s="2">
+        <v>8</v>
+      </c>
+      <c r="D165" s="3">
+        <v>286</v>
+      </c>
+      <c r="E165" s="3">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5">
+      <c r="A166" t="s">
+        <v>8</v>
+      </c>
+      <c r="B166" s="2">
+        <v>2023</v>
+      </c>
+      <c r="C166" s="2">
+        <v>9</v>
+      </c>
+      <c r="D166" s="3">
+        <v>270</v>
+      </c>
+      <c r="E166" s="3">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5">
+      <c r="A167" t="s">
+        <v>8</v>
+      </c>
+      <c r="B167" s="2">
+        <v>2023</v>
+      </c>
+      <c r="C167" s="2">
+        <v>10</v>
+      </c>
+      <c r="D167" s="3">
+        <v>266</v>
+      </c>
+      <c r="E167" s="3">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5">
+      <c r="A168" t="s">
+        <v>8</v>
+      </c>
+      <c r="B168" s="2">
+        <v>2023</v>
+      </c>
+      <c r="C168" s="2">
+        <v>11</v>
+      </c>
+      <c r="D168" s="3">
+        <v>275</v>
+      </c>
+      <c r="E168" s="3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5">
+      <c r="A169" t="s">
+        <v>8</v>
+      </c>
+      <c r="B169" s="2">
+        <v>2023</v>
+      </c>
+      <c r="C169" s="2">
+        <v>12</v>
+      </c>
+      <c r="D169" s="3">
+        <v>266</v>
+      </c>
+      <c r="E169" s="3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5">
+      <c r="A170" t="s">
+        <v>8</v>
+      </c>
+      <c r="B170" s="2">
+        <v>2024</v>
+      </c>
+      <c r="C170" s="2">
+        <v>1</v>
+      </c>
+      <c r="D170" s="3">
+        <v>249</v>
+      </c>
+      <c r="E170" s="3">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5">
+      <c r="A171" t="s">
+        <v>8</v>
+      </c>
+      <c r="B171" s="2">
+        <v>2024</v>
+      </c>
+      <c r="C171" s="2">
+        <v>2</v>
+      </c>
+      <c r="D171" s="3">
+        <v>291</v>
+      </c>
+      <c r="E171" s="3">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5">
+      <c r="A172" t="s">
+        <v>8</v>
+      </c>
+      <c r="B172" s="2">
+        <v>2024</v>
+      </c>
+      <c r="C172" s="2">
+        <v>3</v>
+      </c>
+      <c r="D172" s="3">
+        <v>314</v>
+      </c>
+      <c r="E172" s="3">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5">
+      <c r="A173" t="s">
+        <v>8</v>
+      </c>
+      <c r="B173" s="2">
+        <v>2024</v>
+      </c>
+      <c r="C173" s="2">
+        <v>4</v>
+      </c>
+      <c r="D173" s="3">
+        <v>266</v>
+      </c>
+      <c r="E173" s="3">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5">
+      <c r="A174" t="s">
+        <v>8</v>
+      </c>
+      <c r="B174" s="2">
+        <v>2024</v>
+      </c>
+      <c r="C174" s="2">
+        <v>5</v>
+      </c>
+      <c r="D174" s="3">
+        <v>283</v>
+      </c>
+      <c r="E174" s="3">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5">
+      <c r="A175" t="s">
+        <v>8</v>
+      </c>
+      <c r="B175" s="2">
+        <v>2024</v>
+      </c>
+      <c r="C175" s="2">
+        <v>6</v>
+      </c>
+      <c r="D175" s="3">
+        <v>253</v>
+      </c>
+      <c r="E175" s="3">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5">
+      <c r="A176" t="s">
+        <v>8</v>
+      </c>
+      <c r="B176" s="2">
+        <v>2024</v>
+      </c>
+      <c r="C176" s="2">
+        <v>7</v>
+      </c>
+      <c r="D176" s="3">
+        <v>248</v>
+      </c>
+      <c r="E176" s="3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5">
+      <c r="A177" t="s">
+        <v>8</v>
+      </c>
+      <c r="B177" s="2">
+        <v>2024</v>
+      </c>
+      <c r="C177" s="2">
+        <v>8</v>
+      </c>
+      <c r="D177" s="3">
+        <v>254</v>
+      </c>
+      <c r="E177" s="3">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5">
+      <c r="A178" t="s">
+        <v>8</v>
+      </c>
+      <c r="B178" s="2">
+        <v>2024</v>
+      </c>
+      <c r="C178" s="2">
+        <v>9</v>
+      </c>
+      <c r="D178" s="3">
+        <v>268</v>
+      </c>
+      <c r="E178" s="3">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5">
+      <c r="A179" t="s">
+        <v>8</v>
+      </c>
+      <c r="B179" s="2">
+        <v>2024</v>
+      </c>
+      <c r="C179" s="2">
+        <v>10</v>
+      </c>
+      <c r="D179" s="3">
+        <v>254</v>
+      </c>
+      <c r="E179" s="3">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5">
+      <c r="A180" t="s">
+        <v>8</v>
+      </c>
+      <c r="B180" s="2">
+        <v>2024</v>
+      </c>
+      <c r="C180" s="2">
+        <v>11</v>
+      </c>
+      <c r="D180" s="3">
+        <v>216</v>
+      </c>
+      <c r="E180" s="3">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5">
+      <c r="A181" t="s">
+        <v>8</v>
+      </c>
+      <c r="B181" s="2">
+        <v>2024</v>
+      </c>
+      <c r="C181" s="2">
+        <v>12</v>
+      </c>
+      <c r="D181" s="3">
+        <v>235</v>
+      </c>
+      <c r="E181" s="3">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5">
+      <c r="A182" t="s">
+        <v>8</v>
+      </c>
+      <c r="B182" s="2">
+        <v>2025</v>
+      </c>
+      <c r="C182" s="2">
+        <v>1</v>
+      </c>
+      <c r="D182" s="3">
+        <v>282</v>
+      </c>
+      <c r="E182" s="3">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5">
+      <c r="A183" t="s">
+        <v>8</v>
+      </c>
+      <c r="B183" s="2">
+        <v>2025</v>
+      </c>
+      <c r="C183" s="2">
+        <v>2</v>
+      </c>
+      <c r="D183" s="3">
+        <v>242</v>
+      </c>
+      <c r="E183" s="3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5">
+      <c r="A184" t="s">
+        <v>8</v>
+      </c>
+      <c r="B184" s="2">
+        <v>2025</v>
+      </c>
+      <c r="C184" s="2">
+        <v>3</v>
+      </c>
+      <c r="D184" s="3">
+        <v>296</v>
+      </c>
+      <c r="E184" s="3">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5">
+      <c r="A185" t="s">
+        <v>8</v>
+      </c>
+      <c r="B185" s="2">
+        <v>2025</v>
+      </c>
+      <c r="C185" s="2">
+        <v>4</v>
+      </c>
+      <c r="D185" s="3">
+        <v>296</v>
+      </c>
+      <c r="E185" s="3">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5">
+      <c r="A186" t="s">
+        <v>8</v>
+      </c>
+      <c r="B186" s="2">
+        <v>2025</v>
+      </c>
+      <c r="C186" s="2">
+        <v>5</v>
+      </c>
+      <c r="D186" s="3">
+        <v>296</v>
+      </c>
+      <c r="E186" s="3">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5">
+      <c r="A187" t="s">
+        <v>8</v>
+      </c>
+      <c r="B187" s="2">
+        <v>2025</v>
+      </c>
+      <c r="C187" s="2">
+        <v>6</v>
+      </c>
+      <c r="D187" s="3">
+        <v>286</v>
+      </c>
+      <c r="E187" s="3">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="188" spans="1:5">
+      <c r="A188" t="s">
+        <v>8</v>
+      </c>
+      <c r="B188" s="2">
+        <v>2025</v>
+      </c>
+      <c r="C188" s="2">
+        <v>7</v>
+      </c>
+      <c r="D188" s="3">
+        <v>255</v>
+      </c>
+      <c r="E188" s="3">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5">
+      <c r="A189" t="s">
+        <v>8</v>
+      </c>
+      <c r="B189" s="2">
+        <v>2025</v>
+      </c>
+      <c r="C189" s="2">
+        <v>8</v>
+      </c>
+      <c r="D189" s="3">
+        <v>262</v>
+      </c>
+      <c r="E189" s="3">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5">
+      <c r="A190" t="s">
+        <v>8</v>
+      </c>
+      <c r="B190" s="2">
+        <v>2025</v>
+      </c>
+      <c r="C190" s="2">
+        <v>9</v>
+      </c>
+      <c r="D190" s="3">
+        <v>248</v>
+      </c>
+      <c r="E190" s="3">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5">
+      <c r="A191" t="s">
+        <v>8</v>
+      </c>
+      <c r="B191" s="2">
+        <v>2025</v>
+      </c>
+      <c r="C191" s="2">
+        <v>10</v>
+      </c>
+      <c r="D191" s="3">
+        <v>266</v>
+      </c>
+      <c r="E191" s="3">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5">
+      <c r="A192" t="s">
+        <v>8</v>
+      </c>
+      <c r="B192" s="2">
+        <v>2025</v>
+      </c>
+      <c r="C192" s="2">
+        <v>11</v>
+      </c>
+      <c r="D192" s="3">
         <v>246</v>
       </c>
-      <c r="E45" s="3">
+      <c r="E192" s="3">
         <v>87</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5">
+      <c r="A193" t="s">
+        <v>8</v>
+      </c>
+      <c r="B193" s="2">
+        <v>2025</v>
+      </c>
+      <c r="C193" s="2">
+        <v>12</v>
+      </c>
+      <c r="D193" s="3">
+        <v>250</v>
+      </c>
+      <c r="E193" s="3">
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>